<commit_message>
updated capacitors because they were out of stock
</commit_message>
<xml_diff>
--- a/Buylist/Windprobe_Test_Lab_Shopping_list.xlsx
+++ b/Buylist/Windprobe_Test_Lab_Shopping_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHischier\Documents\GitHub\Weatherstation\Buylist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F764AB-3473-4B5B-9CBA-403F387C1ADC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D915EF-9C8E-4633-9CA6-C552C2F283A2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33060" yWindow="2805" windowWidth="21600" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4695" yWindow="1665" windowWidth="21600" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>Designation</t>
   </si>
@@ -114,9 +114,6 @@
     <t>https://www.amazon.fr/BOJACK-condensateurs-monolithiques-c%C3%A9ramique-Capacit%C3%A9/dp/B07PP7SFY8/ref=pd_bxgy_328_img_2/257-6635116-7314721?_encoding=UTF8&amp;pd_rd_i=B07PP7SFY8&amp;pd_rd_r=a33e17f7-ad5c-4ed8-ac9f-093307b207f0&amp;pd_rd_w=w9n4R&amp;pd_rd_wg=LaEy1&amp;pf_rd_p=6f987254-9a2f-416c-82f5-9555ce4bf24d&amp;pf_rd_r=BSC7EJKK86G9VXGEZPQ5&amp;psc=1&amp;refRID=BSC7EJKK86G9VXGEZPQ5</t>
   </si>
   <si>
-    <t>https://www.amazon.fr/BOJACK-dassortiment-condensateur-%C3%A9lectrolytique-0-1uF-1000uF/dp/B07PN5P64W/ref=sxbs_sxwds-stvp?__mk_fr_FR=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;keywords=condensateur+MKP+lot&amp;pd_rd_i=B07PN5P64W&amp;pd_rd_r=7e2db12e-5b14-4f19-8c0b-82a6a0b510d5&amp;pd_rd_w=NLFep&amp;pd_rd_wg=MkfY0&amp;pf_rd_p=b5ee69d3-6381-4897-8a23-e5b0b965bfb9&amp;pf_rd_r=A3B3BG0V87ASFRAFGBTW&amp;qid=1576586658&amp;s=industrial</t>
-  </si>
-  <si>
     <t>Polarized capacitor high capacity</t>
   </si>
   <si>
@@ -160,6 +157,12 @@
   </si>
   <si>
     <t>Meteo station</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/Wandefol-Condensateur-Electrolytique-Rangement-Valeurs/dp/B07Q6PNB6H/</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -513,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G18"/>
+  <dimension ref="B2:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,13 +551,13 @@
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3" s="1">
         <v>89.9</v>
@@ -572,7 +575,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4">
         <v>0.4</v>
@@ -624,7 +627,7 @@
         <v>11.99</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -635,17 +638,17 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7">
+        <v>15.95</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>15.95</v>
+      </c>
+      <c r="G7" t="s">
         <v>27</v>
-      </c>
-      <c r="E7">
-        <v>18.989999999999998</v>
-      </c>
-      <c r="F7" s="2">
-        <f t="shared" si="0"/>
-        <v>18.989999999999998</v>
-      </c>
-      <c r="G7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -656,7 +659,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E8">
         <v>0.8</v>
@@ -698,7 +701,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10">
         <v>104.9</v>
@@ -719,7 +722,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11">
         <v>18.399999999999999</v>
@@ -791,7 +794,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E15">
         <v>30.79</v>
@@ -803,13 +806,13 @@
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E16">
         <v>29</v>
@@ -821,13 +824,13 @@
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E17">
         <v>6.99</v>
@@ -839,13 +842,13 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="E18">
         <v>10.199999999999999</v>
@@ -853,6 +856,15 @@
       <c r="F18" s="2">
         <f t="shared" si="0"/>
         <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="2">
+        <f>SUM(F3:F18)</f>
+        <v>462.16</v>
       </c>
     </row>
   </sheetData>
@@ -863,7 +875,7 @@
     <hyperlink ref="D14" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="D5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="D6" r:id="rId6" display="https://www.amazon.fr/BOJACK-condensateurs-monolithiques-c%C3%A9ramique-Capacit%C3%A9/dp/B07PP7SFY8/ref=pd_bxgy_328_img_2/257-6635116-7314721?_encoding=UTF8&amp;pd_rd_i=B07PP7SFY8&amp;pd_rd_r=a33e17f7-ad5c-4ed8-ac9f-093307b207f0&amp;pd_rd_w=w9n4R&amp;pd_rd_wg=LaEy1&amp;pf_rd_p=6f987254-9a2f-416c-82f5-9555ce4bf24d&amp;pf_rd_r=BSC7EJKK86G9VXGEZPQ5&amp;psc=1&amp;refRID=BSC7EJKK86G9VXGEZPQ5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="D7" r:id="rId7" display="https://www.amazon.fr/BOJACK-dassortiment-condensateur-%C3%A9lectrolytique-0-1uF-1000uF/dp/B07PN5P64W/ref=sxbs_sxwds-stvp?__mk_fr_FR=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;keywords=condensateur+MKP+lot&amp;pd_rd_i=B07PN5P64W&amp;pd_rd_r=7e2db12e-5b14-4f19-8c0b-82a6a0b510d5&amp;pd_rd_w=NLFep&amp;pd_rd_wg=MkfY0&amp;pf_rd_p=b5ee69d3-6381-4897-8a23-e5b0b965bfb9&amp;pf_rd_r=A3B3BG0V87ASFRAFGBTW&amp;qid=1576586658&amp;s=industrial" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="D16" r:id="rId8" display="https://www.amazon.fr/Pi-EzConnect-Connecteur-Raspberry-connecter-Pi-3/dp/B01FE9EQ88/ref=pd_sbs_107_8?_encoding=UTF8&amp;pd_rd_i=B01FE9EQ88&amp;pd_rd_r=99f7a7e3-dd61-4d79-8fc9-4450ecf584db&amp;pd_rd_w=joAWD&amp;pd_rd_wg=mFIuN&amp;pf_rd_p=a9f5d7c2-08ef-42e9-9709-9c2a12683b28&amp;pf_rd_r=Q8EFM19GHCTBEQHWE13E&amp;psc=1&amp;refRID=Q8EFM19GHCTBEQHWE13E" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="D17" r:id="rId9" display="https://www.amazon.fr/DollaTek-Carte-dextension-Breakout-Raspberry/dp/B07DK4XDLW/ref=pd_sbs_107_9?_encoding=UTF8&amp;pd_rd_i=B07DK4XDLW&amp;pd_rd_r=99f7a7e3-dd61-4d79-8fc9-4450ecf584db&amp;pd_rd_w=joAWD&amp;pd_rd_wg=mFIuN&amp;pf_rd_p=a9f5d7c2-08ef-42e9-9709-9c2a12683b28&amp;pf_rd_r=Q8EFM19GHCTBEQHWE13E&amp;psc=1&amp;refRID=Q8EFM19GHCTBEQHWE13E" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="D15" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
@@ -880,21 +892,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F33C1526C759B14BB410FD12855095B5" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="19eecc58f349faf6d004235fc186344b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9d871e14-6b06-4ec1-b75e-a6fbb5a6e734" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2b74170313794ca59e5797bb5160e5af" ns2:_="">
     <xsd:import namespace="9d871e14-6b06-4ec1-b75e-a6fbb5a6e734"/>
@@ -1064,31 +1061,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{750AFB1A-9C24-4F32-909A-FC833B038C1C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9d871e14-6b06-4ec1-b75e-a6fbb5a6e734"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1421E826-2DBF-4AC2-8C26-D9905DCCE1CC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{144FF5B1-02D2-4FC6-8932-579B8761EC2E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1104,4 +1092,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1421E826-2DBF-4AC2-8C26-D9905DCCE1CC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{750AFB1A-9C24-4F32-909A-FC833B038C1C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9d871e14-6b06-4ec1-b75e-a6fbb5a6e734"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>